<commit_message>
Grids implementation for center the button
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C6FD35-7454-4077-8383-00AB841F19FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77C3958-69A4-454F-939E-56DD4C459C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Plans</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>make target column as a drop down menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klib library implementation </t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,10 +429,18 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>